<commit_message>
Resistence Transfer and Demo development
</commit_message>
<xml_diff>
--- a/Game Info spread sheet.xlsx
+++ b/Game Info spread sheet.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="195">
   <si>
     <t>Creature Type</t>
   </si>
@@ -209,9 +209,6 @@
     <t>Rage Demon</t>
   </si>
   <si>
-    <t>Terrifing Bunny of The Pit</t>
-  </si>
-  <si>
     <t>Demon of The Forge</t>
   </si>
   <si>
@@ -467,18 +464,12 @@
     <t>Unlike shades the banshee can adapt to any eviorment, without being corrupted. This banshee has the attributes of fire and shadow.</t>
   </si>
   <si>
-    <t>These spirits literaly poured their souls into their creations, so munch so that upon its completion they died.</t>
-  </si>
-  <si>
     <t>Corruption</t>
   </si>
   <si>
     <t>water</t>
   </si>
   <si>
-    <t>Soon after its body's death the soul was captured and tortured for centeries in the relm of Wastes, before being unlessed upon the world.</t>
-  </si>
-  <si>
     <t>All who have been consumed by the mist either become one with it or are warpped into a mindless Wasteland creature.</t>
   </si>
   <si>
@@ -621,6 +612,18 @@
   </si>
   <si>
     <t>transfer</t>
+  </si>
+  <si>
+    <t>Terrifying Bunny of The Pit</t>
+  </si>
+  <si>
+    <t>Soon after its body's death the soul was captured and tortured for centeries in the realm of Wastes, before being unleashed upon the world.</t>
+  </si>
+  <si>
+    <t>In life, these spirits literaly poured their souls into their creations, so munch so that upon its completion they died.</t>
+  </si>
+  <si>
+    <t>resistence</t>
   </si>
 </sst>
 </file>
@@ -957,7 +960,7 @@
   <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,15 +973,21 @@
         <v>15</v>
       </c>
       <c r="N1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q1" t="s">
         <v>30</v>
       </c>
+      <c r="R1" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="Q2" t="s">
-        <v>193</v>
+        <v>190</v>
+      </c>
+      <c r="R2" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -986,7 +995,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G3" t="s">
         <v>16</v>
@@ -995,10 +1004,13 @@
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q3" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="R3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1006,7 +1018,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G4" t="s">
         <v>17</v>
@@ -1015,10 +1027,13 @@
         <v>2</v>
       </c>
       <c r="P4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q4" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="R4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -1026,7 +1041,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G5" t="s">
         <v>18</v>
@@ -1035,10 +1050,13 @@
         <v>3</v>
       </c>
       <c r="P5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q5" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="R5" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1046,7 +1064,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G6" t="s">
         <v>19</v>
@@ -1055,10 +1073,13 @@
         <v>4</v>
       </c>
       <c r="P6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q6" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="R6" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1066,7 +1087,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G7" t="s">
         <v>20</v>
@@ -1075,10 +1096,13 @@
         <v>5</v>
       </c>
       <c r="P7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q7" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="R7" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -1086,7 +1110,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G8" t="s">
         <v>21</v>
@@ -1095,10 +1119,13 @@
         <v>6</v>
       </c>
       <c r="P8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q8" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="R8" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1106,16 +1133,19 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N9" t="s">
         <v>7</v>
       </c>
       <c r="P9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q9" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="R9" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -1123,16 +1153,19 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N10" t="s">
         <v>8</v>
       </c>
       <c r="P10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q10" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="R10" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -1140,16 +1173,19 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N11" t="s">
         <v>9</v>
       </c>
       <c r="P11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q11" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="R11" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -1157,19 +1193,19 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N12" t="s">
         <v>10</v>
       </c>
       <c r="P12" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="Q12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -1177,16 +1213,19 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q13" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="R13" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -1194,16 +1233,19 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N14" t="s">
         <v>12</v>
       </c>
       <c r="P14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q14" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="R14" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -1211,16 +1253,19 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N15" t="s">
         <v>13</v>
       </c>
       <c r="P15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q15" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="R15" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -1228,16 +1273,19 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N16" t="s">
         <v>14</v>
       </c>
       <c r="P16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q16" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="R16" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1257,7 +1305,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1288,7 +1336,7 @@
         <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E5">
         <v>240</v>
@@ -1297,13 +1345,13 @@
         <v>52</v>
       </c>
       <c r="I5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K5" t="s">
         <v>52</v>
       </c>
       <c r="M5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1328,7 +1376,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1359,7 +1407,7 @@
         <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E5">
         <v>384</v>
@@ -1368,13 +1416,13 @@
         <v>52</v>
       </c>
       <c r="I5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K5" t="s">
         <v>52</v>
       </c>
       <c r="M5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1382,7 +1430,7 @@
         <v>53</v>
       </c>
       <c r="M6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1390,33 +1438,33 @@
         <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E8">
         <v>3795</v>
       </c>
       <c r="G8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M8" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I9" t="s">
         <v>13</v>
       </c>
       <c r="M9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -1436,7 +1484,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1467,7 +1515,7 @@
         <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E5">
         <v>380</v>
@@ -1482,12 +1530,12 @@
         <v>53</v>
       </c>
       <c r="M5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1507,7 +1555,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1533,7 +1581,7 @@
         <v>31</v>
       </c>
       <c r="O3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1541,22 +1589,22 @@
         <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E5">
         <v>438</v>
       </c>
       <c r="G5" t="s">
+        <v>133</v>
+      </c>
+      <c r="I5" t="s">
         <v>134</v>
-      </c>
-      <c r="I5" t="s">
-        <v>135</v>
       </c>
       <c r="K5" t="s">
         <v>13</v>
       </c>
       <c r="M5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1576,7 +1624,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1607,22 +1655,22 @@
         <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E5">
         <v>516</v>
       </c>
       <c r="G5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K5" t="s">
         <v>13</v>
       </c>
       <c r="M5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1642,7 +1690,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1673,7 +1721,7 @@
         <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E5">
         <v>590</v>
@@ -1682,21 +1730,21 @@
         <v>52</v>
       </c>
       <c r="I5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K5" t="s">
         <v>13</v>
       </c>
       <c r="M5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1796,16 +1844,16 @@
         <v>680</v>
       </c>
       <c r="F5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H5" t="s">
         <v>13</v>
       </c>
       <c r="J5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
@@ -1819,18 +1867,18 @@
         <v>52</v>
       </c>
       <c r="H7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
@@ -1847,10 +1895,10 @@
         <v>53</v>
       </c>
       <c r="J9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
@@ -1861,21 +1909,21 @@
         <v>5671</v>
       </c>
       <c r="F11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D13">
         <v>7362</v>
@@ -1884,13 +1932,13 @@
         <v>53</v>
       </c>
       <c r="H13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
@@ -1904,22 +1952,22 @@
         <v>8590</v>
       </c>
       <c r="F15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L15" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q15" t="s">
         <v>147</v>
       </c>
-      <c r="Q15" t="s">
-        <v>150</v>
-      </c>
       <c r="Y15" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1932,7 +1980,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1979,18 +2027,18 @@
         <v>52</v>
       </c>
       <c r="I5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K5" t="s">
         <v>52</v>
       </c>
       <c r="M5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2001,21 +2049,21 @@
         <v>482</v>
       </c>
       <c r="G7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K7" t="s">
         <v>52</v>
       </c>
       <c r="M7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -2026,16 +2074,16 @@
         <v>394</v>
       </c>
       <c r="G9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K9" t="s">
         <v>52</v>
       </c>
       <c r="M9" t="s">
-        <v>145</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -2055,7 +2103,7 @@
         <v>53</v>
       </c>
       <c r="M11" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -2074,13 +2122,13 @@
         <v>52</v>
       </c>
       <c r="I13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K13" t="s">
         <v>13</v>
       </c>
       <c r="M13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2094,7 +2142,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2141,13 +2189,13 @@
         <v>53</v>
       </c>
       <c r="I5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K5" t="s">
         <v>52</v>
       </c>
       <c r="M5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2161,24 +2209,24 @@
         <v>52</v>
       </c>
       <c r="I7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K7" t="s">
         <v>52</v>
       </c>
       <c r="M7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>56</v>
+        <v>191</v>
       </c>
       <c r="E9">
         <v>800</v>
       </c>
       <c r="G9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I9" t="s">
         <v>52</v>
@@ -2187,12 +2235,12 @@
         <v>52</v>
       </c>
       <c r="M9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E11">
         <v>656</v>
@@ -2201,13 +2249,13 @@
         <v>13</v>
       </c>
       <c r="I11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K11" t="s">
         <v>52</v>
       </c>
       <c r="M11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -2215,7 +2263,7 @@
         <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E13">
         <v>830</v>
@@ -2230,27 +2278,27 @@
         <v>53</v>
       </c>
       <c r="M13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E15">
         <v>2300</v>
       </c>
       <c r="G15" t="s">
+        <v>113</v>
+      </c>
+      <c r="I15" t="s">
         <v>114</v>
       </c>
-      <c r="I15" t="s">
+      <c r="K15" t="s">
+        <v>58</v>
+      </c>
+      <c r="M15" t="s">
         <v>115</v>
-      </c>
-      <c r="K15" t="s">
-        <v>59</v>
-      </c>
-      <c r="M15" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2301,7 +2349,7 @@
         <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5">
         <v>150</v>
@@ -2310,23 +2358,23 @@
         <v>52</v>
       </c>
       <c r="I5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K5" t="s">
         <v>52</v>
       </c>
       <c r="M5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E8">
         <v>300</v>
@@ -2335,38 +2383,38 @@
         <v>53</v>
       </c>
       <c r="I8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K8" t="s">
         <v>52</v>
       </c>
       <c r="M8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E11">
         <v>520</v>
       </c>
       <c r="G11" t="s">
+        <v>122</v>
+      </c>
+      <c r="I11" t="s">
+        <v>64</v>
+      </c>
+      <c r="K11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M11" t="s">
         <v>123</v>
-      </c>
-      <c r="I11" t="s">
-        <v>65</v>
-      </c>
-      <c r="K11" t="s">
-        <v>52</v>
-      </c>
-      <c r="M11" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -2374,7 +2422,7 @@
         <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E13">
         <v>3500</v>
@@ -2383,18 +2431,18 @@
         <v>52</v>
       </c>
       <c r="I13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K13" t="s">
         <v>53</v>
       </c>
       <c r="M13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E15">
         <v>48527</v>
@@ -2403,18 +2451,18 @@
         <v>13</v>
       </c>
       <c r="I15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2466,7 +2514,7 @@
         <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E5">
         <v>500</v>
@@ -2475,23 +2523,23 @@
         <v>52</v>
       </c>
       <c r="I5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K5" t="s">
         <v>52</v>
       </c>
       <c r="M5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E7">
         <v>260</v>
@@ -2500,26 +2548,26 @@
         <v>52</v>
       </c>
       <c r="I7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K7" t="s">
         <v>52</v>
       </c>
       <c r="M7" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="M8" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E10">
         <v>290</v>
@@ -2528,24 +2576,24 @@
         <v>52</v>
       </c>
       <c r="I10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K10" t="s">
         <v>52</v>
       </c>
       <c r="M10" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E12">
         <v>349</v>
       </c>
       <c r="G12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I12" t="s">
         <v>13</v>
@@ -2554,12 +2602,12 @@
         <v>52</v>
       </c>
       <c r="M12" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E14">
         <v>100</v>
@@ -2568,13 +2616,13 @@
         <v>53</v>
       </c>
       <c r="I14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K14" t="s">
         <v>53</v>
       </c>
       <c r="M14" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -2582,12 +2630,12 @@
         <v>52</v>
       </c>
       <c r="M15" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E17">
         <v>382</v>
@@ -2596,18 +2644,18 @@
         <v>13</v>
       </c>
       <c r="I17" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="K17" t="s">
         <v>13</v>
       </c>
       <c r="M17" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E19">
         <v>670</v>
@@ -2616,13 +2664,13 @@
         <v>52</v>
       </c>
       <c r="I19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K19" t="s">
         <v>13</v>
       </c>
       <c r="M19" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -2630,7 +2678,7 @@
         <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E21">
         <v>3000</v>
@@ -2639,23 +2687,23 @@
         <v>52</v>
       </c>
       <c r="I21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K21" t="s">
         <v>52</v>
       </c>
       <c r="M21" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M22" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E24">
         <v>780</v>
@@ -2664,13 +2712,13 @@
         <v>52</v>
       </c>
       <c r="I24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K24" t="s">
         <v>53</v>
       </c>
       <c r="M24" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -2678,32 +2726,32 @@
         <v>53</v>
       </c>
       <c r="M25" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E27">
         <v>873600</v>
       </c>
       <c r="G27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M27" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E29">
         <v>1780</v>
@@ -2718,12 +2766,12 @@
         <v>13</v>
       </c>
       <c r="M29" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2774,22 +2822,22 @@
         <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E5">
         <v>930</v>
       </c>
       <c r="G5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K5" t="s">
         <v>52</v>
       </c>
       <c r="M5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2799,7 +2847,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E7">
         <v>845</v>
@@ -2814,12 +2862,12 @@
         <v>52</v>
       </c>
       <c r="M7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E9">
         <v>937</v>
@@ -2834,7 +2882,7 @@
         <v>52</v>
       </c>
       <c r="M9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -2842,27 +2890,27 @@
         <v>43</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E11">
         <v>7140</v>
       </c>
       <c r="G11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M11" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2883,7 +2931,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -2897,7 +2945,7 @@
         <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I3" t="s">
         <v>29</v>
@@ -2931,16 +2979,16 @@
         <v>52</v>
       </c>
       <c r="I7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M7" t="s">
         <v>52</v>
       </c>
       <c r="O7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -2954,7 +3002,7 @@
         <v>53</v>
       </c>
       <c r="I9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K9" t="s">
         <v>52</v>
@@ -2965,25 +3013,25 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E11">
         <v>613540</v>
       </c>
       <c r="G11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I11" t="s">
         <v>52</v>
       </c>
       <c r="K11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O11" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2994,19 +3042,19 @@
         <v>52130</v>
       </c>
       <c r="G13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I13" t="s">
         <v>53</v>
       </c>
       <c r="K13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="M13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O13" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -3017,27 +3065,27 @@
         <v>17850</v>
       </c>
       <c r="G15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I15" t="s">
         <v>13</v>
       </c>
       <c r="K15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -3057,7 +3105,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -3088,7 +3136,7 @@
         <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5">
         <v>315</v>
@@ -3097,13 +3145,13 @@
         <v>52</v>
       </c>
       <c r="I5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K5" t="s">
         <v>52</v>
       </c>
       <c r="M5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -3113,13 +3161,13 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E7">
         <v>130</v>
       </c>
       <c r="G7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I7" t="s">
         <v>52</v>
@@ -3128,37 +3176,37 @@
         <v>53</v>
       </c>
       <c r="M7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M8" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E10">
         <v>220</v>
       </c>
       <c r="G10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K10" t="s">
         <v>53</v>
       </c>
       <c r="M10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E12">
         <v>400</v>
@@ -3167,13 +3215,13 @@
         <v>53</v>
       </c>
       <c r="I12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K12" t="s">
         <v>53</v>
       </c>
       <c r="M12" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -3181,7 +3229,7 @@
         <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E14">
         <v>4740</v>
@@ -3190,18 +3238,18 @@
         <v>52</v>
       </c>
       <c r="I14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K14" t="s">
         <v>52</v>
       </c>
       <c r="M14" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E16">
         <v>13846</v>
@@ -3210,21 +3258,21 @@
         <v>13</v>
       </c>
       <c r="I16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M16" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M17" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>